<commit_message>
Add complete GUI and app structure
</commit_message>
<xml_diff>
--- a/OFAC_2025-02-26.xlsx
+++ b/OFAC_2025-02-26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,29 +433,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="44" customWidth="1" min="1" max="1"/>
-    <col width="69" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="9" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="69" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID OFAC</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Nombre Completo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Documentos</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Alias</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Accion</t>
         </is>
@@ -464,20 +470,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>52752</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>YONGHONGAN TRADE LIMITED</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>['Business Registration Number 74682749', 'Company Number 3216131']</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>add</t>
         </is>
@@ -486,20 +497,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>52753</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>DINGTAI INDUSTRIAL TECHNOLOGY CO LIMITED</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>['Business Registration Number 68310851', 'Company Number 2590461']</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>add</t>
         </is>
@@ -508,20 +524,25 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>52754</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>HONG KONG TIANLE INTERNATIONAL CO LIMITED</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>['Business Registration Number 71502619', 'Company Number 2906297']</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>add</t>
         </is>
@@ -530,20 +551,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>52755</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>DDC DEVELOP INDUSTRY HONG KONG LIMITED</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>['Business Registration Number 71234020', 'Company Number 2879836']</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>add</t>
         </is>
@@ -552,20 +578,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>52756</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>SHENZHEN ZHIYU INTERNATIONAL TRADE CO LTD</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>['Unified Social Credit Code (USCC) 91440300MADHXGM776']</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>add</t>
         </is>
@@ -574,20 +605,25 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>52757</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>JP ORIENTAL INTERNATIONAL HOLDINGS LIMITED</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>['Business Registration Number 33802039', 'Company Number 0821175']</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>add</t>
         </is>

</xml_diff>